<commit_message>
# Data modifications for further tests
</commit_message>
<xml_diff>
--- a/Correction_nom_cellule/cellules_coleo_CD.xlsx
+++ b/Correction_nom_cellule/cellules_coleo_CD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP_9470m\Desktop\PostDoc_COLEO\GitHub\rcoleo_Extras\Correction_nom_cellule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B09AAF33-58A0-449F-BF84-12C892412888}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{06C73CCE-B29D-4DF1-975B-CDE71D231C51}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="4320" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -725,7 +725,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -908,6 +908,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1072,9 +1078,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1433,7 +1440,7 @@
   <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+      <selection activeCell="D61" activeCellId="1" sqref="D49 D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,16 +1659,16 @@
       <c r="B15">
         <v>18</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1895,16 +1902,16 @@
       <c r="B30">
         <v>102</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="1" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1915,16 +1922,16 @@
       <c r="B31">
         <v>119</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2068,84 +2075,88 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="1">
         <v>115</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>390</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="1">
         <v>116</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>446</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="G42" s="1"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="1">
         <v>117</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>495</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="G43" s="1"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="1">
         <v>118</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>574</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -2231,7 +2242,7 @@
       <c r="C49" t="s">
         <v>141</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E49" t="s">
@@ -2425,7 +2436,7 @@
       <c r="C61" t="s">
         <v>137</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="2" t="s">
         <v>142</v>
       </c>
       <c r="E61">

</xml_diff>